<commit_message>
a few changes, need to test the actual outcome formula to perfect the parameters m and x
</commit_message>
<xml_diff>
--- a/resources/method_comparisons.xlsx
+++ b/resources/method_comparisons.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jack.amy\mfm_libraries\eloCalc\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C723054B-FC1B-4750-9D7A-4ABBEF370036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EDFB976-3863-484C-B6A2-2C9EC2779494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{0B36F180-A65C-4DC6-AE0D-6D034FE3F4C6}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{0B36F180-A65C-4DC6-AE0D-6D034FE3F4C6}"/>
   </bookViews>
   <sheets>
     <sheet name="f1_squashing_f(x)s" sheetId="1" r:id="rId1"/>
+    <sheet name="actual_outcome" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,8 +36,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Algebraic</t>
   </si>
@@ -58,15 +81,40 @@
   <si>
     <t>Base</t>
   </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>ActualOutcomeAlgebraic</t>
+  </si>
+  <si>
+    <t>ActualOutcomeLogistic</t>
+  </si>
+  <si>
+    <t>=$H$1+0.5-($H$1^(1+B2/$H$2))</t>
+  </si>
+  <si>
+    <t>$H$1+0.5-($H$1^(1+C2/$H$2))</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -92,8 +140,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1428,7 +1478,1573 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>actual_outcome!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ActualOutcomeLogistic</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>actual_outcome!$A$2:$A$76</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="75"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0472251898884349E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0966805983368683E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1484715478402893E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2027083347685118E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.259506464258358E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.3189868961986701E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.3812763028320097E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.4465073385216467E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.514818922258346E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.5863565335085907E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.661272522034293E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.7397264323438019E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.8218853434651669E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.9079242247652659E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.9980263085725508E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.0923834803969775E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.1911966875781494E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.2946763672319369E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.4030428944069687E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.5165270514053924E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.6353705192673944E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.7598263924661807E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.8901597179095108E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.026648059395692E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.1695820887261167E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.3192662047331893E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.4760191815419783E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3.6401748474461405E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.8120827958438894E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3.9921091297480532E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4.1806372414557584E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4.378068629038169E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4.5848237513890971E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4.8013429236534538E-2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>5.0280872549424808E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>5.2655396303327585E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>5.5142057392403021E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>5.7746151523598216E-2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>6.0473224494626478E-2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>6.3329084004551173E-2</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>6.6319812022126751E-2</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>6.9451777738236964E-2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>7.2731651130014591E-2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>7.6166417165528938E-2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>7.9763390679292778E-2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>8.3530231950267819E-2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>8.7474963015544221E-2</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>9.1605984754437098E-2</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>9.5932094779382457E-2</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.10046250617173409</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.10520686710236228</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.11017528137883872</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.11537832996296611</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.12082709350447766</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.12653317593889432</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.13250872919979534</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.13876647909813092</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.14531975242368966</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.15218250532643871</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.15936935303817759</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.16689560099780246</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.17477727744646809</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.18303116756206131</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.19167484920568154</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.20072673035625693</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.2102060883130159</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.22013311074930317</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.23052893870517097</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.24141571161030201</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.25281661443315007</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.26475592705670692</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.27725907598604849</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.29035268849778145</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.30406464934670685</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>actual_outcome!$E$2:$E$76</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="75"/>
+                <c:pt idx="0">
+                  <c:v>0.22135759971146976</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.22132614210255433</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.22129320419474183</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.22125871661720706</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.22122260677862263</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.2211847987209824</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.22114521296717146</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.22110376636206364</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.22106037190692349</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.22101493858689053</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.22096737119132281</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.22091757012678101</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.22086543122243593</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.22081084552768968</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.22075369910180861</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.22069387279537447</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.2206312420233795</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.22056567652980091</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.22049704014351917</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.22042519052546464</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.22034997890691177</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.22027124981887708</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.22018884081262083</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.22010258217130593</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.22001229661292862</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.21991779898470917</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.21981889594921233</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.21971538566256882</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.21960705744527734</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.21949369144620154</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.21937505830052378</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.21925091878258926</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.21912102345477349</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.21898511231373041</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.21884291443563439</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.21869414762232545</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.21853851805059643</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.2183757199272405</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.21820543515290436</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.21802733299827468</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.21784106979666953</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.21764628865772048</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.2174426192075149</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.21722967736134163</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.21700706513603804</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.21677437050989637</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.21653116733914665</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.21627701534120872</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.21601146015619926</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.21573403349959847</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.2154442534205285</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.21514162468177805</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.21482563927951653</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.21449577712258047</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.21415150689326723</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.21379228711372592</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.21341756744426119</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.21302679024213125</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.2126193924116774</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.21219480757879777</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.21175246862479885</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.21129181061640898</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.21081227417009185</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.21031330928959127</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.20979437971567516</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.20925496782610117</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.20869458012162043</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.20811275333007512</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.20750906115497447</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.20688312168698608</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.20623460548614989</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.20556324432891659</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.20486884059692351</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.20415127726341945</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.20341052840815485</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4CD8-476F-8264-937F7BF1A6BC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="299196127"/>
+        <c:axId val="299195167"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="299196127"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="299195167"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="299195167"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="299196127"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>actual_outcome!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ActualOutcomeAlgebraic</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>actual_outcome!$A$2:$A$76</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="75"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0472251898884349E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0966805983368683E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1484715478402893E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2027083347685118E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.259506464258358E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.3189868961986701E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.3812763028320097E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.4465073385216467E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.514818922258346E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.5863565335085907E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.661272522034293E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.7397264323438019E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.8218853434651669E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.9079242247652659E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.9980263085725508E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.0923834803969775E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.1911966875781494E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.2946763672319369E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.4030428944069687E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.5165270514053924E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.6353705192673944E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.7598263924661807E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.8901597179095108E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.026648059395692E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.1695820887261167E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.3192662047331893E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.4760191815419783E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3.6401748474461405E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.8120827958438894E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3.9921091297480532E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4.1806372414557584E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4.378068629038169E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4.5848237513890971E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4.8013429236534538E-2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>5.0280872549424808E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>5.2655396303327585E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>5.5142057392403021E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>5.7746151523598216E-2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>6.0473224494626478E-2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>6.3329084004551173E-2</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>6.6319812022126751E-2</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>6.9451777738236964E-2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>7.2731651130014591E-2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>7.6166417165528938E-2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>7.9763390679292778E-2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>8.3530231950267819E-2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>8.7474963015544221E-2</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>9.1605984754437098E-2</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>9.5932094779382457E-2</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.10046250617173409</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.10520686710236228</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.11017528137883872</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.11537832996296611</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.12082709350447766</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.12653317593889432</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.13250872919979534</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.13876647909813092</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.14531975242368966</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.15218250532643871</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.15936935303817759</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.16689560099780246</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.17477727744646809</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.18303116756206131</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.19167484920568154</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.20072673035625693</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.2102060883130159</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.22013311074930317</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.23052893870517097</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.24141571161030201</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.25281661443315007</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.26475592705670692</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.27725907598604849</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.29035268849778145</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.30406464934670685</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>actual_outcome!$D$2:$D$76</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="75"/>
+                <c:pt idx="0">
+                  <c:v>0.22202149997444584</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.22202117693114817</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.22202082265637194</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.22202043413074846</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.22202000804301733</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.22201954076180988</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.22201902830470707</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.22201846630430566</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.22201784997100574</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.22201717405220203</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.22201643278753161</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.22201561985979709</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.22201472834114819</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.22201375063406281</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.22201267840662708</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.22201150252156202</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.22201021295839526</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.22200879872811422</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.22200724777957737</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.22200554689688662</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.22200368158685027</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.22200163595558015</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.22199939257317589</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.22199693232534806</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.2219942342507219</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.22199127536244187</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.22198803045256582</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.22198447187759363</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.221980569323313</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.22197628954697601</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.22197159609462702</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.22196644899119586</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.22196080440074209</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.22195461425398852</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.22194782584000888</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.22194038135863833</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.22193221742985075</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.22192326455599057</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.22191344653236308</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.22190267980125999</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.22189087274404215</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.2218779249053934</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.22186372614331909</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.22184815569786348</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.22183108117087655</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.2218123574084602</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.22179182527696073</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.22176931032255437</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.22174462130358041</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.22171754858382092</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.22168786237388935</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.2216553108067881</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.22161961783250811</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.22158048091528504</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.22153756851579065</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.22149051733913061</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.22143892932805076</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.22138236837923012</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.22132035675897913</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.2212523711930971</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.2211778386040909</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.22109613146748927</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.22100656275763989</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.22090838045225722</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.22080076156419295</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.22068280566858481</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.22055352789388794</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.22041185134656099</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.22025659894168656</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.22008648461597022</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.21990010390592749</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.21969592388331624</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.2194722724529018</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.21922732703556977</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.21895910268407939</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-12B1-4D5F-8438-52B839D0860F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="299187967"/>
+        <c:axId val="299190367"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="299187967"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="299190367"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="299190367"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="299187967"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1984,6 +3600,1038 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -2017,6 +4665,83 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>358140</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3665CCB-6B83-EC37-E769-AC0546069992}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>604520</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>299720</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAEE329B-2308-5A0A-627B-0192AF563270}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2344,8 +5069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41D15009-5345-4C6F-AA60-01E9FB9C6B83}">
   <dimension ref="A1:H76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S21" sqref="S21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2373,11 +5098,11 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <f t="shared" ref="B2:B6" si="0">1/(1+EXP(-(A2^2)))</f>
+        <f>1/(1+EXP(-(A2^2)))</f>
         <v>0.7310585786300049</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:C6" si="1">0.5*(1+(A2/(SQRT(1+(A2^2)))))</f>
+        <f t="shared" ref="C2:C6" si="0">0.5*(1+(A2/(SQRT(1+(A2^2)))))</f>
         <v>0.85355339059327373</v>
       </c>
       <c r="G2" t="s">
@@ -2393,11 +5118,11 @@
         <v>1.0472251898884348</v>
       </c>
       <c r="B3">
+        <f t="shared" ref="B2:B6" si="1">1/(1+EXP(-(A3^2)))</f>
+        <v>0.74963763318045062</v>
+      </c>
+      <c r="C3">
         <f t="shared" si="0"/>
-        <v>0.74963763318045062</v>
-      </c>
-      <c r="C3">
-        <f t="shared" si="1"/>
         <v>0.86161292612737594</v>
       </c>
       <c r="G3" t="s">
@@ -2413,11 +5138,11 @@
         <v>1.0966805983368684</v>
       </c>
       <c r="B4">
+        <f t="shared" si="1"/>
+        <v>0.76900623076852115</v>
+      </c>
+      <c r="C4">
         <f t="shared" si="0"/>
-        <v>0.76900623076852115</v>
-      </c>
-      <c r="C4">
-        <f t="shared" si="1"/>
         <v>0.86946360806303091</v>
       </c>
       <c r="G4" t="s">
@@ -2433,11 +5158,11 @@
         <v>1.1484715478402894</v>
       </c>
       <c r="B5">
+        <f t="shared" si="1"/>
+        <v>0.78901310306905992</v>
+      </c>
+      <c r="C5">
         <f t="shared" si="0"/>
-        <v>0.78901310306905992</v>
-      </c>
-      <c r="C5">
-        <f t="shared" si="1"/>
         <v>0.87708659805165023</v>
       </c>
     </row>
@@ -2447,11 +5172,11 @@
         <v>1.2027083347685117</v>
       </c>
       <c r="B6">
+        <f t="shared" si="1"/>
+        <v>0.80946032792108846</v>
+      </c>
+      <c r="C6">
         <f t="shared" si="0"/>
-        <v>0.80946032792108846</v>
-      </c>
-      <c r="C6">
-        <f t="shared" si="1"/>
         <v>0.88446522476401057</v>
       </c>
     </row>
@@ -3311,7 +6036,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68">
-        <f t="shared" ref="A68:A106" si="5">$H$4^($H$1+ (ROW()-ROW($A$2))*($H$2-$H$1)/($H$3-1))</f>
+        <f t="shared" ref="A68:A76" si="5">$H$4^($H$1+ (ROW()-ROW($A$2))*($H$2-$H$1)/($H$3-1))</f>
         <v>21.02060883130159</v>
       </c>
       <c r="B68">
@@ -3371,11 +6096,11 @@
         <v>25.281661443315009</v>
       </c>
       <c r="B72">
-        <f t="shared" ref="B72:B106" si="6">1/(1+EXP(-(A72^2)))</f>
+        <f t="shared" ref="B72:B76" si="6">1/(1+EXP(-(A72^2)))</f>
         <v>1</v>
       </c>
       <c r="C72">
-        <f t="shared" ref="C72:C106" si="7">0.5*(1+(A72/(SQRT(1+(A72^2)))))</f>
+        <f t="shared" ref="C72:C76" si="7">0.5*(1+(A72/(SQRT(1+(A72^2)))))</f>
         <v>0.99960932146948811</v>
       </c>
     </row>
@@ -3433,6 +6158,1633 @@
       <c r="C76">
         <f t="shared" si="7"/>
         <v>0.99972981824485352</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D795AB3-6FCC-420A-B0FB-ECBDCB948D6C}">
+  <dimension ref="A1:H76"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" cm="1">
+        <f t="array" ref="A2:A76">'f1_squashing_f(x)s'!A2:A76/100</f>
+        <v>0.01</v>
+      </c>
+      <c r="B2">
+        <f>1/(1+EXP(-(A2^2)))</f>
+        <v>0.50002499999997918</v>
+      </c>
+      <c r="C2">
+        <f>0.5*(1+(A2/(SQRT(1+(A2^2)))))</f>
+        <v>0.50499975001874842</v>
+      </c>
+      <c r="D2">
+        <f>($H$1^(1+B2/$H$2))</f>
+        <v>0.22202149997444584</v>
+      </c>
+      <c r="E2">
+        <f>($H$1^(1+C2/$H$2))</f>
+        <v>0.22135759971146976</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>1.0472251898884349E-2</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B66" si="0">1/(1+EXP(-(A3^2)))</f>
+        <v>0.50002741701493103</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C66" si="1">0.5*(1+(A3/(SQRT(1+(A3^2)))))</f>
+        <v>0.50523583885516876</v>
+      </c>
+      <c r="D3">
+        <f>($H$1^(1+B3/$H$2))</f>
+        <v>0.22202117693114817</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E66" si="2">($H$1^(1+C3/$H$2))</f>
+        <v>0.22132614210255433</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>1.0966805983368683E-2</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>0.50003006770833291</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="1"/>
+        <v>0.50548307327470154</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D67" si="3">($H$1^(1+B4/$H$2))</f>
+        <v>0.22202082265637194</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="2"/>
+        <v>0.22129320419474183</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>1.1484715478402893E-2</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>0.50003297467235719</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="1"/>
+        <v>0.50574197907192975</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="3"/>
+        <v>0.22202043413074846</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="2"/>
+        <v>0.22125871661720706</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>1.2027083347685118E-2</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>0.50003616268340001</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>0.50601310678941369</v>
+      </c>
+      <c r="D6">
+        <f>($H$1^(1+B6/$H$2))</f>
+        <v>0.22202000804301733</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="2"/>
+        <v>0.22122260677862263</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>1.259506464258358E-2</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>0.50003965891325453</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>0.50629703287413641</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="3"/>
+        <v>0.22201954076180988</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="2"/>
+        <v>0.2211847987209824</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>1.3189868961986701E-2</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>0.50004349316069896</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>0.5065943608867427</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="3"/>
+        <v>0.22201902830470707</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="2"/>
+        <v>0.22114521296717146</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>1.3812763028320097E-2</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>0.50004769810547445</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>0.50690572276579193</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="3"/>
+        <v>0.22201846630430566</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="2"/>
+        <v>0.22110376636206364</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>1.4465073385216467E-2</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>0.50005230958681912</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>0.50723178014931469</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="3"/>
+        <v>0.22201784997100574</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="2"/>
+        <v>0.22106037190692349</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>1.514818922258346E-2</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>0.5000573669089291</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>0.50757322575602415</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="3"/>
+        <v>0.22201717405220203</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="2"/>
+        <v>0.22101493858689053</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>1.5863565335085907E-2</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>0.50006291317595308</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>0.50793078482858822</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="3"/>
+        <v>0.22201643278753161</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="2"/>
+        <v>0.22096737119132281</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>1.661272522034293E-2</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>0.50006899565937368</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>0.5083052166414288</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="3"/>
+        <v>0.22201561985979709</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="2"/>
+        <v>0.22091757012678101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>1.7397264323438019E-2</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>0.50007566620090727</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>0.50869731607555357</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="3"/>
+        <v>0.22201472834114819</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="2"/>
+        <v>0.22086543122243593</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>1.8218853434651669E-2</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>0.5000829816543565</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>0.50910791526297206</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="3"/>
+        <v>0.22201375063406281</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="2"/>
+        <v>0.22081084552768968</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>1.9079242247652659E-2</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>0.50009100437018117</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="1"/>
+        <v>0.50953788530327027</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="3"/>
+        <v>0.22201267840662708</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="2"/>
+        <v>0.22075369910180861</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>1.9980263085725508E-2</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>0.50009980272691823</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>0.50998813805494247</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="3"/>
+        <v>0.22201150252156202</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="2"/>
+        <v>0.22069387279537447</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>2.0923834803969775E-2</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>0.50010945171397769</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="1"/>
+        <v>0.51045962800407418</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="3"/>
+        <v>0.22201021295839526</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="2"/>
+        <v>0.2206312420233795</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>2.1911966875781494E-2</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>0.50012003357078538</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="1"/>
+        <v>0.51095335421296106</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="3"/>
+        <v>0.22200879872811422</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="2"/>
+        <v>0.22056567652980091</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>2.2946763672319369E-2</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>0.5001316384877168</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="1"/>
+        <v>0.51147036235121113</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="3"/>
+        <v>0.22200724777957737</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="2"/>
+        <v>0.22049704014351917</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>2.4030428944069687E-2</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>0.50014436537479723</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="1"/>
+        <v>0.51201174681181538</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="3"/>
+        <v>0.22200554689688662</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="2"/>
+        <v>0.22042519052546464</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>2.5165270514053924E-2</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>0.50015832270472005</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="1"/>
+        <v>0.51257865291458693</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="3"/>
+        <v>0.22200368158685027</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="2"/>
+        <v>0.22034997890691177</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>2.6353705192673944E-2</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>0.50017362943736632</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="1"/>
+        <v>0.51317227919923925</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="3"/>
+        <v>0.22200163595558015</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="2"/>
+        <v>0.22027124981887708</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>2.7598263924661807E-2</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>0.50019041603370828</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="1"/>
+        <v>0.51379387981021474</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="3"/>
+        <v>0.22199939257317589</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="2"/>
+        <v>0.22018884081262083</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>2.8901597179095108E-2</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>0.50020882556773372</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="1"/>
+        <v>0.51444476697516051</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="3"/>
+        <v>0.22199693232534806</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="2"/>
+        <v>0.22010258217130593</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>3.026648059395692E-2</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>0.50022901494587102</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="1"/>
+        <v>0.5151263135786821</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="3"/>
+        <v>0.2219942342507219</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="2"/>
+        <v>0.22001229661292862</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>3.1695820887261167E-2</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>0.50025115624430561</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="1"/>
+        <v>0.51583995583267639</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="3"/>
+        <v>0.22199127536244187</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="2"/>
+        <v>0.21991779898470917</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>3.3192662047331893E-2</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>0.50027543817558517</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="1"/>
+        <v>0.51658719604413839</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="3"/>
+        <v>0.22198803045256582</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="2"/>
+        <v>0.21981889594921233</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>3.4760191815419783E-2</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>0.50030206769701169</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="1"/>
+        <v>0.51736960548084487</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="3"/>
+        <v>0.22198447187759363</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="2"/>
+        <v>0.21971538566256882</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>3.6401748474461405E-2</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>0.5003312717745273</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="1"/>
+        <v>0.51818882733473015</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="3"/>
+        <v>0.221980569323313</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="2"/>
+        <v>0.21960705744527734</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>3.8120827958438894E-2</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>0.50036329931712509</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="1"/>
+        <v>0.51904657978205793</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="3"/>
+        <v>0.22197628954697601</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="2"/>
+        <v>0.21949369144620154</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>3.9921091297480532E-2</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="0"/>
+        <v>0.50039842329826723</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="1"/>
+        <v>0.51994465913866006</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="3"/>
+        <v>0.22197159609462702</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="2"/>
+        <v>0.21937505830052378</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>4.1806372414557584E-2</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="0"/>
+        <v>0.5004369430823884</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="1"/>
+        <v>0.52088494310751732</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="3"/>
+        <v>0.22196644899119586</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="2"/>
+        <v>0.21925091878258926</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>4.378068629038169E-2</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="0"/>
+        <v>0.50047918697630611</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="1"/>
+        <v>0.52186939411479483</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="3"/>
+        <v>0.22196080440074209</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="2"/>
+        <v>0.21912102345477349</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>4.5848237513890971E-2</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="0"/>
+        <v>0.50052551502727649</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="1"/>
+        <v>0.52290006272907574</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="3"/>
+        <v>0.22195461425398852</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="2"/>
+        <v>0.21898511231373041</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>4.8013429236534538E-2</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="0"/>
+        <v>0.50057632209153113</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="1"/>
+        <v>0.52397909115694319</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="3"/>
+        <v>0.22194782584000888</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="2"/>
+        <v>0.21884291443563439</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>5.0280872549424808E-2</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="0"/>
+        <v>0.5006320411994355</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="1"/>
+        <v>0.5251087168062003</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="3"/>
+        <v>0.22194038135863833</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="2"/>
+        <v>0.21869414762232545</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>5.2655396303327585E-2</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="0"/>
+        <v>0.50069314724593161</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="1"/>
+        <v>0.52629127590586355</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="3"/>
+        <v>0.22193221742985075</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="2"/>
+        <v>0.21853851805059643</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>5.5142057392403021E-2</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="0"/>
+        <v>0.5007601610376925</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="1"/>
+        <v>0.5275292071695673</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="3"/>
+        <v>0.22192326455599057</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="2"/>
+        <v>0.2183757199272405</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>5.7746151523598216E-2</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="0"/>
+        <v>0.50083365373144995</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="1"/>
+        <v>0.52882505548613556</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="3"/>
+        <v>0.22191344653236308</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="2"/>
+        <v>0.21820543515290436</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>6.0473224494626478E-2</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="0"/>
+        <v>0.50091425170128179</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="1"/>
+        <v>0.53018147561775841</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="3"/>
+        <v>0.22190267980125999</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="2"/>
+        <v>0.21802733299827468</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>6.3329084004551173E-2</v>
+      </c>
+      <c r="B42">
+        <f t="shared" si="0"/>
+        <v>0.50100264187628185</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="1"/>
+        <v>0.53160123588239783</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="3"/>
+        <v>0.22189087274404215</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="2"/>
+        <v>0.21784106979666953</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>6.6319812022126751E-2</v>
+      </c>
+      <c r="B43">
+        <f t="shared" si="0"/>
+        <v>0.50109957759403445</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="1"/>
+        <v>0.53308722179267543</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="3"/>
+        <v>0.2218779249053934</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="2"/>
+        <v>0.21764628865772048</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>6.9451777738236964E-2</v>
+      </c>
+      <c r="B44">
+        <f t="shared" si="0"/>
+        <v>0.501205885019678</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="1"/>
+        <v>0.53464243961850255</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="3"/>
+        <v>0.22186372614331909</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="2"/>
+        <v>0.2174426192075149</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>7.2731651130014591E-2</v>
+      </c>
+      <c r="B45">
+        <f t="shared" si="0"/>
+        <v>0.50132247018513909</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="1"/>
+        <v>0.53627001983501033</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="3"/>
+        <v>0.22184815569786348</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="2"/>
+        <v>0.21722967736134163</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>7.6166417165528938E-2</v>
+      </c>
+      <c r="B46">
+        <f t="shared" si="0"/>
+        <v>0.50145032670835621</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="1"/>
+        <v>0.53797322041085993</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="3"/>
+        <v>0.22183108117087655</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="2"/>
+        <v>0.21700706513603804</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>7.9763390679292778E-2</v>
+      </c>
+      <c r="B47">
+        <f t="shared" si="0"/>
+        <v>0.50159054425805416</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="1"/>
+        <v>0.53975542988465441</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="3"/>
+        <v>0.2218123574084602</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="2"/>
+        <v>0.21677437050989637</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>8.3530231950267819E-2</v>
+      </c>
+      <c r="B48">
+        <f t="shared" si="0"/>
+        <v>0.50174431783591211</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="1"/>
+        <v>0.54162017016885544</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="3"/>
+        <v>0.22179182527696073</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="2"/>
+        <v>0.21653116733914665</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>8.7474963015544221E-2</v>
+      </c>
+      <c r="B49">
+        <f t="shared" si="0"/>
+        <v>0.50191295795483548</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="1"/>
+        <v>0.54357109901121903</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="3"/>
+        <v>0.22176931032255437</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="2"/>
+        <v>0.21627701534120872</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>9.1605984754437098E-2</v>
+      </c>
+      <c r="B50">
+        <f t="shared" si="0"/>
+        <v>0.50209790179955271</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="1"/>
+        <v>0.54561201203321008</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="3"/>
+        <v>0.22174462130358041</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="2"/>
+        <v>0.21601146015619926</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>9.5932094779382457E-2</v>
+      </c>
+      <c r="B51">
+        <f t="shared" si="0"/>
+        <v>0.50230072546396143</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="1"/>
+        <v>0.54774684425302334</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="3"/>
+        <v>0.22171754858382092</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="2"/>
+        <v>0.21573403349959847</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>0.10046250617173409</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="0"/>
+        <v>0.50252315736860242</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="1"/>
+        <v>0.54997967098764011</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="3"/>
+        <v>0.22168786237388935</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="2"/>
+        <v>0.2154442534205285</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>0.10520686710236228</v>
+      </c>
+      <c r="B53">
+        <f t="shared" si="0"/>
+        <v>0.50276709297140487</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="1"/>
+        <v>0.552314708013665</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="3"/>
+        <v>0.2216553108067881</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="2"/>
+        <v>0.21514162468177805</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>0.11017528137883872</v>
+      </c>
+      <c r="B54">
+        <f t="shared" si="0"/>
+        <v>0.50303461089548052</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="1"/>
+        <v>0.55475631085045496</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="3"/>
+        <v>0.22161961783250811</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="2"/>
+        <v>0.21482563927951653</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <v>0.11537832996296611</v>
+      </c>
+      <c r="B55">
+        <f t="shared" si="0"/>
+        <v>0.50332799060931233</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="1"/>
+        <v>0.55730897301118054</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="3"/>
+        <v>0.22158048091528504</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="2"/>
+        <v>0.21449577712258047</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A56">
+        <v>0.12082709350447766</v>
+      </c>
+      <c r="B56">
+        <f t="shared" si="0"/>
+        <v>0.50364973180723682</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="1"/>
+        <v>0.55997732304792136</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="3"/>
+        <v>0.22153756851579065</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="2"/>
+        <v>0.21415150689326723</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A57">
+        <v>0.12653317593889432</v>
+      </c>
+      <c r="B57">
+        <f t="shared" si="0"/>
+        <v>0.50400257565172712</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="1"/>
+        <v>0.56276612019567318</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="3"/>
+        <v>0.22149051733913061</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="2"/>
+        <v>0.21379228711372592</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A58">
+        <v>0.13250872919979534</v>
+      </c>
+      <c r="B58">
+        <f t="shared" si="0"/>
+        <v>0.50438952805367343</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="1"/>
+        <v>0.56568024839728914</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="3"/>
+        <v>0.22143892932805076</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="2"/>
+        <v>0.21341756744426119</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A59">
+        <v>0.13876647909813092</v>
+      </c>
+      <c r="B59">
+        <f t="shared" si="0"/>
+        <v>0.50481388518268633</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="1"/>
+        <v>0.56872470846700129</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="3"/>
+        <v>0.22138236837923012</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="2"/>
+        <v>0.21302679024213125</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A60">
+        <v>0.14531975242368966</v>
+      </c>
+      <c r="B60">
+        <f t="shared" si="0"/>
+        <v>0.50527926141641166</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="1"/>
+        <v>0.57190460812447041</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="3"/>
+        <v>0.22132035675897913</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="2"/>
+        <v>0.2126193924116774</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A61">
+        <v>0.15218250532643871</v>
+      </c>
+      <c r="B61">
+        <f t="shared" si="0"/>
+        <v>0.50578961995594696</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="1"/>
+        <v>0.57522514960461446</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="3"/>
+        <v>0.2212523711930971</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="2"/>
+        <v>0.21219480757879777</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A62">
+        <v>0.15936935303817759</v>
+      </c>
+      <c r="B62">
+        <f t="shared" si="0"/>
+        <v>0.50634930635362707</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="1"/>
+        <v>0.57869161452122664</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="3"/>
+        <v>0.2211778386040909</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="2"/>
+        <v>0.21175246862479885</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A63">
+        <v>0.16689560099780246</v>
+      </c>
+      <c r="B63">
+        <f t="shared" si="0"/>
+        <v>0.5069630852195931</v>
+      </c>
+      <c r="C63">
+        <f t="shared" si="1"/>
+        <v>0.5823093456352505</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="3"/>
+        <v>0.22109613146748927</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="2"/>
+        <v>0.21129181061640898</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A64">
+        <v>0.17477727744646809</v>
+      </c>
+      <c r="B64">
+        <f t="shared" si="0"/>
+        <v>0.50763618039449043</v>
+      </c>
+      <c r="C64">
+        <f t="shared" si="1"/>
+        <v>0.5860837251523916</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="3"/>
+        <v>0.22100656275763989</v>
+      </c>
+      <c r="E64">
+        <f t="shared" si="2"/>
+        <v>0.21081227417009185</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A65">
+        <v>0.18303116756206131</v>
+      </c>
+      <c r="B65">
+        <f t="shared" si="0"/>
+        <v>0.50837431889705909</v>
+      </c>
+      <c r="C65">
+        <f t="shared" si="1"/>
+        <v>0.59002014915062084</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="3"/>
+        <v>0.22090838045225722</v>
+      </c>
+      <c r="E65">
+        <f t="shared" si="2"/>
+        <v>0.21031330928959127</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A66">
+        <v>0.19167484920568154</v>
+      </c>
+      <c r="B66">
+        <f t="shared" si="0"/>
+        <v>0.5091837789768473</v>
+      </c>
+      <c r="C66">
+        <f t="shared" si="1"/>
+        <v>0.5941239977174968</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="3"/>
+        <v>0.22080076156419295</v>
+      </c>
+      <c r="E66">
+        <f t="shared" si="2"/>
+        <v>0.20979437971567516</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A67">
+        <v>0.20072673035625693</v>
+      </c>
+      <c r="B67">
+        <f t="shared" ref="B67:B76" si="4">1/(1+EXP(-(A67^2)))</f>
+        <v>0.51007144262315618</v>
+      </c>
+      <c r="C67">
+        <f t="shared" ref="C67:C76" si="5">0.5*(1+(A67/(SQRT(1+(A67^2)))))</f>
+        <v>0.59840060036187548</v>
+      </c>
+      <c r="D67">
+        <f t="shared" si="3"/>
+        <v>0.22068280566858481</v>
+      </c>
+      <c r="E67">
+        <f t="shared" ref="E67:E76" si="6">($H$1^(1+C67/$H$2))</f>
+        <v>0.20925496782610117</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A68">
+        <v>0.2102060883130159</v>
+      </c>
+      <c r="B68">
+        <f t="shared" si="4"/>
+        <v>0.51104485290071577</v>
+      </c>
+      <c r="C68">
+        <f t="shared" si="5"/>
+        <v>0.60285519625666151</v>
+      </c>
+      <c r="D68">
+        <f t="shared" ref="D68:D76" si="7">($H$1^(1+B68/$H$2))</f>
+        <v>0.22055352789388794</v>
+      </c>
+      <c r="E68">
+        <f t="shared" si="6"/>
+        <v>0.20869458012162043</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A69">
+        <v>0.22013311074930317</v>
+      </c>
+      <c r="B69">
+        <f t="shared" si="4"/>
+        <v>0.51211227649923552</v>
+      </c>
+      <c r="C69">
+        <f t="shared" si="5"/>
+        <v>0.60749288887142938</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="7"/>
+        <v>0.22041185134656099</v>
+      </c>
+      <c r="E69">
+        <f t="shared" si="6"/>
+        <v>0.20811275333007512</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A70">
+        <v>0.23052893870517097</v>
+      </c>
+      <c r="B70">
+        <f t="shared" si="4"/>
+        <v>0.51328277189616356</v>
+      </c>
+      <c r="C70">
+        <f t="shared" si="5"/>
+        <v>0.61231859456909088</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="7"/>
+        <v>0.22025659894168656</v>
+      </c>
+      <c r="E70">
+        <f t="shared" si="6"/>
+        <v>0.20750906115497447</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A71">
+        <v>0.24141571161030201</v>
+      </c>
+      <c r="B71">
+        <f t="shared" si="4"/>
+        <v>0.51456626353736623</v>
+      </c>
+      <c r="C71">
+        <f t="shared" si="5"/>
+        <v>0.61733698477291465</v>
+      </c>
+      <c r="D71">
+        <f t="shared" si="7"/>
+        <v>0.22008648461597022</v>
+      </c>
+      <c r="E71">
+        <f t="shared" si="6"/>
+        <v>0.20688312168698608</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A72">
+        <v>0.25281661443315007</v>
+      </c>
+      <c r="B72">
+        <f t="shared" si="4"/>
+        <v>0.51597362243584388</v>
+      </c>
+      <c r="C72">
+        <f t="shared" si="5"/>
+        <v>0.62255242136319011</v>
+      </c>
+      <c r="D72">
+        <f t="shared" si="7"/>
+        <v>0.21990010390592749</v>
+      </c>
+      <c r="E72">
+        <f t="shared" si="6"/>
+        <v>0.20623460548614989</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A73">
+        <v>0.26475592705670692</v>
+      </c>
+      <c r="B73">
+        <f t="shared" si="4"/>
+        <v>0.51751675356979621</v>
+      </c>
+      <c r="C73">
+        <f t="shared" si="5"/>
+        <v>0.62796888504115511</v>
+      </c>
+      <c r="D73">
+        <f t="shared" si="7"/>
+        <v>0.21969592388331624</v>
+      </c>
+      <c r="E73">
+        <f t="shared" si="6"/>
+        <v>0.20556324432891659</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A74">
+        <v>0.27725907598604849</v>
+      </c>
+      <c r="B74">
+        <f t="shared" si="4"/>
+        <v>0.51920869042264717</v>
+      </c>
+      <c r="C74">
+        <f t="shared" si="5"/>
+        <v>0.63358989650630781</v>
+      </c>
+      <c r="D74">
+        <f t="shared" si="7"/>
+        <v>0.2194722724529018</v>
+      </c>
+      <c r="E74">
+        <f t="shared" si="6"/>
+        <v>0.20486884059692351</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A75">
+        <v>0.29035268849778145</v>
+      </c>
+      <c r="B75">
+        <f t="shared" si="4"/>
+        <v>0.52106369694153187</v>
+      </c>
+      <c r="C75">
+        <f t="shared" si="5"/>
+        <v>0.63941843043682856</v>
+      </c>
+      <c r="D75">
+        <f t="shared" si="7"/>
+        <v>0.21922732703556977</v>
+      </c>
+      <c r="E75">
+        <f t="shared" si="6"/>
+        <v>0.20415127726341945</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A76">
+        <v>0.30406464934670685</v>
+      </c>
+      <c r="B76">
+        <f t="shared" si="4"/>
+        <v>0.52309737708727388</v>
+      </c>
+      <c r="C76">
+        <f t="shared" si="5"/>
+        <v>0.6454568224463636</v>
+      </c>
+      <c r="D76">
+        <f t="shared" si="7"/>
+        <v>0.21895910268407939</v>
+      </c>
+      <c r="E76">
+        <f t="shared" si="6"/>
+        <v>0.20341052840815485</v>
       </c>
     </row>
   </sheetData>

</xml_diff>